<commit_message>
New changes 24th April, 2021 around 11PM IST
</commit_message>
<xml_diff>
--- a/RestAssuredTestCase1.xlsx
+++ b/RestAssuredTestCase1.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14100" windowHeight="3708"/>
   </bookViews>
   <sheets>
-    <sheet name="Rest Assured - Test  Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Rest Assured - Test  Cases" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -222,6 +223,30 @@
   </si>
   <si>
     <t>VVK07_GET_Request_Autherization</t>
+  </si>
+  <si>
+    <t>EMPNAME</t>
+  </si>
+  <si>
+    <t>TEST123</t>
+  </si>
+  <si>
+    <t>TEST124</t>
+  </si>
+  <si>
+    <t>TEST125</t>
+  </si>
+  <si>
+    <t>TEST126</t>
+  </si>
+  <si>
+    <t>TEST127</t>
+  </si>
+  <si>
+    <t>EMPSAL</t>
+  </si>
+  <si>
+    <t>EMPAGE</t>
   </si>
 </sst>
 </file>
@@ -260,7 +285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +301,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -351,6 +382,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -633,9 +673,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="16">
+        <v>50000</v>
+      </c>
+      <c r="C2" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="16">
+        <v>60000</v>
+      </c>
+      <c r="C3" s="16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="16">
+        <v>70000</v>
+      </c>
+      <c r="C4" s="16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="16">
+        <v>80000</v>
+      </c>
+      <c r="C5" s="16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="16">
+        <v>90000</v>
+      </c>
+      <c r="C6" s="16">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>